<commit_message>
Changed shares outstanding measure
</commit_message>
<xml_diff>
--- a/Book values.xlsx
+++ b/Book values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Meistaraverkefni\DCL_coco_bond\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steinarb20\Desktop\DCL_coco_bond\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701B333C-90AA-4CFA-8E4B-53BBC3B07C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F15A75-84E3-4504-BD19-238F88CF0644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5478CA7-EC92-43C0-B583-E08DEE665488}"/>
+    <workbookView xWindow="3570" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{D5478CA7-EC92-43C0-B583-E08DEE665488}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance sheet" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Steinar Björnsson</author>
     <author>Lenovo</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{78F45D7F-979D-430D-B62C-09B3399223A9}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{9DC3D75E-9E23-4323-9556-5615801310DA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steinar Björnsson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+From form 20-f filings</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="1" shapeId="0" xr:uid="{78F45D7F-979D-430D-B62C-09B3399223A9}">
       <text>
         <r>
           <rPr>
@@ -67,15 +92,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{91F591BD-43B4-4E3F-883F-BAE32047098A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steinar Björnsson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.finma.ch/en/news/2023/03/20230323-mm-at1-kapitalinstrumente/#:~:text=US225401AS71%20,down%20Capital%20Notes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{6A8E63A4-DAB3-46D1-BD45-139CEB01DB11}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steinar Björnsson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.finma.ch/en/news/2023/03/20230323-mm-at1-kapitalinstrumente/#:~:text=US225401AS71%20,down%20Capital%20Notes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{14B4EB23-6C31-43E5-91D4-9C73DAEBF606}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steinar Björnsson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.finma.ch/en/news/2023/03/20230323-mm-at1-kapitalinstrumente/#:~:text=US225401AS71%20,down%20Capital%20Notes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{04611D16-D44F-4A2A-926F-96ADC1056077}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Steinar Björnsson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.finma.ch/en/news/2023/03/20230323-mm-at1-kapitalinstrumente/#:~:text=US225401AS71%20,down%20Capital%20Notes</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
-  <si>
-    <t>Shares outstanding</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Bank</t>
   </si>
@@ -104,9 +222,6 @@
     <t>AT1 drawdown gain</t>
   </si>
   <si>
-    <t>AT1 capital instruments</t>
-  </si>
-  <si>
     <t>Form 6k:</t>
   </si>
   <si>
@@ -143,17 +258,27 @@
     <t>Write down - perpetual contingent capital notes</t>
   </si>
   <si>
-    <t>(Atricles say 17 billion? Is this from convertin to USD?)</t>
+    <t>AT1 issuances</t>
+  </si>
+  <si>
+    <t>(see notes)</t>
+  </si>
+  <si>
+    <t>Debt/Assets</t>
+  </si>
+  <si>
+    <t>No significant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +314,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,12 +347,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -243,8 +382,8 @@
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>513423</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>532473</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>34775</xdr:rowOff>
     </xdr:to>
@@ -287,8 +426,8 @@
       <xdr:rowOff>154305</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>159093</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>349593</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>91608</xdr:rowOff>
     </xdr:to>
@@ -419,8 +558,8 @@
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>3002</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22052</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>72776</xdr:rowOff>
     </xdr:to>
@@ -824,55 +963,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AAFA7C-3C87-4636-9B65-BAE28EB68682}">
-  <dimension ref="B1:I48"/>
+  <dimension ref="B2:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="2">
         <v>2018</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2019</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>2020</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>2021</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>2022</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>2550600000</v>
@@ -891,9 +1023,9 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>4399680200</v>
@@ -914,7 +1046,7 @@
         <v>4399680200</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -922,36 +1054,41 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>3</v>
+      </c>
       <c r="H7" s="1">
         <f>16*10^9</f>
         <v>16000000000</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10216000000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>13017000000</v>
+      </c>
+      <c r="E8" s="1">
+        <v>15841000000</v>
+      </c>
+      <c r="F8" s="1">
+        <v>15844000000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>14736000000</v>
+      </c>
       <c r="H8" s="1">
         <v>15007000000</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -962,100 +1099,143 @@
         <v>14113000000</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H11" s="1"/>
-      <c r="I11">
-        <f>H8/H13</f>
-        <v>3.6214589602573413E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43922000000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43644000000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>42677000000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>43954000000</v>
+      </c>
       <c r="G12" s="1">
         <v>48476000000</v>
       </c>
       <c r="H12" s="1">
-        <v>38116000000</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+        <v>37655000000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>724897000000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>758115000000</v>
+      </c>
+      <c r="E13" s="1">
+        <v>776024000000</v>
+      </c>
+      <c r="F13" s="1">
+        <v>711603000000</v>
+      </c>
       <c r="G13" s="1">
-        <v>481663000000</v>
+        <v>481563000000</v>
       </c>
       <c r="H13" s="1">
         <v>414391000000</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ref="C14:F14" si="0">C13+C12</f>
-        <v>0</v>
+        <v>768819000000</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>801759000000</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>818701000000</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>755557000000</v>
       </c>
       <c r="G14" s="1">
         <f>G13+G12</f>
-        <v>530139000000</v>
+        <v>530039000000</v>
       </c>
       <c r="H14" s="1">
         <f>H13+H12</f>
-        <v>452507000000</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
+        <v>452046000000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3">
+        <f>C13/C14</f>
+        <v>0.94287081874927647</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ref="D15:H15" si="1">D13/D14</f>
+        <v>0.94556468963865703</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.94787230014376433</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.94182569945086869</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.90854257894230428</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.91670095521252259</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1">
-        <v>1200000000</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1063,7 +1243,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1071,15 +1251,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1087,7 +1259,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1095,7 +1267,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1103,7 +1275,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1111,7 +1283,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1119,7 +1291,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1127,7 +1299,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1135,7 +1307,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1143,7 +1315,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1151,7 +1323,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1159,9 +1331,9 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1180,245 +1352,245 @@
       <selection activeCell="M8" sqref="M8:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="12:15" x14ac:dyDescent="0.25">
       <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+    </row>
+    <row r="3" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
         <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="12:15" x14ac:dyDescent="0.3">
-      <c r="L3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="12:15" x14ac:dyDescent="0.3">
-      <c r="M4" t="s">
-        <v>16</v>
       </c>
       <c r="N4" s="1">
         <v>700000000</v>
       </c>
     </row>
-    <row r="5" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N5" s="1">
         <f>SUM(N4)</f>
         <v>700000000</v>
       </c>
     </row>
-    <row r="7" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="12:15" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="12:15" x14ac:dyDescent="0.25">
       <c r="M8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N8" s="1">
         <v>125000000</v>
       </c>
     </row>
-    <row r="9" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L9" s="2"/>
       <c r="M9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N9" s="1">
         <v>175000000</v>
       </c>
     </row>
-    <row r="10" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L10" s="2"/>
       <c r="M10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N10" s="1">
         <v>1050000000</v>
       </c>
     </row>
-    <row r="11" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L11" s="2"/>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N11" s="1">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="12" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L12" s="2"/>
       <c r="M12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N12" s="1">
         <v>2000000000</v>
       </c>
     </row>
-    <row r="13" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L13" s="2"/>
       <c r="M13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N13" s="1">
         <v>2500000000</v>
       </c>
     </row>
-    <row r="14" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N14" s="1">
         <f>SUM(N8:N13)</f>
         <v>6850000000</v>
       </c>
     </row>
-    <row r="16" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="12:14" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N17" s="1">
         <v>300000000</v>
       </c>
     </row>
-    <row r="18" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L18" s="2"/>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N18" s="1">
         <v>200000000</v>
       </c>
     </row>
-    <row r="19" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L19" s="2"/>
       <c r="M19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N19" s="1">
         <v>525000000</v>
       </c>
     </row>
-    <row r="20" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L20" s="2"/>
       <c r="M20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N20" s="1">
         <v>1500000000</v>
       </c>
     </row>
-    <row r="21" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L21" s="2"/>
       <c r="M21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N21" s="1">
         <v>1500000000</v>
       </c>
     </row>
-    <row r="22" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L22" s="2"/>
       <c r="M22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N22" s="1">
         <v>750000000</v>
       </c>
     </row>
-    <row r="23" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L23" s="2"/>
       <c r="M23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N23" s="1">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="24" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L24" s="2"/>
       <c r="M24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N24" s="1">
         <v>2500000000</v>
       </c>
     </row>
-    <row r="25" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L25" s="2"/>
       <c r="M25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N25" s="1">
         <v>1750000000</v>
       </c>
     </row>
-    <row r="26" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L26" s="2"/>
       <c r="M26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N26" s="1">
         <v>2250000000</v>
       </c>
     </row>
-    <row r="27" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L27" s="2"/>
       <c r="M27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N27" s="1">
         <v>2000000000</v>
       </c>
     </row>
-    <row r="28" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L28" s="2"/>
       <c r="M28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N28" s="1">
         <v>1500000000</v>
       </c>
     </row>
-    <row r="29" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L29" s="2"/>
       <c r="M29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N29" s="1">
         <v>1650000000</v>
       </c>
     </row>
-    <row r="30" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N30" s="1">
         <f>SUM(N17:N29)</f>
         <v>17425000000</v>
       </c>
     </row>
-    <row r="32" spans="12:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N32" s="1">
         <f>N5+N14+N30</f>

</xml_diff>